<commit_message>
Update repository with latest changes: optimization outputs, new results, paper and presentation materials
</commit_message>
<xml_diff>
--- a/CMA framework/Excel files/Alternatives.xlsx
+++ b/CMA framework/Excel files/Alternatives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gigan\OneDrive\Desktop\NYU\Fall 2025\Capstone\CMA framework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{317BFF54-8DA0-4D02-8815-0CCEDFA503A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F00F36F-7367-433C-8319-BCC2FC7CECA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="761" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="private_equity" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -6501,7 +6501,7 @@
       <selection activeCell="E273" sqref="E273"/>
       <selection pane="topRight" activeCell="E273" sqref="E273"/>
       <selection pane="bottomLeft" activeCell="E273" sqref="E273"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -39071,7 +39071,7 @@
   </sheetPr>
   <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D13" sqref="D13:J14"/>
     </sheetView>
   </sheetViews>
@@ -39240,8 +39240,8 @@
   </sheetPr>
   <dimension ref="B2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update repository with latest changes: new company SVGs, updated optimization files, paper and presentation versions, and framework updates
</commit_message>
<xml_diff>
--- a/CMA framework/Excel files/Alternatives.xlsx
+++ b/CMA framework/Excel files/Alternatives.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gigan\OneDrive\Desktop\NYU\Fall 2025\Capstone\CMA framework\Excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F00F36F-7367-433C-8319-BCC2FC7CECA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44ECC814-71CB-4BB9-9D46-7C6BB301BE83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="761" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="761" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="private_equity" sheetId="1" r:id="rId1"/>
@@ -6214,8 +6214,8 @@
   </sheetPr>
   <dimension ref="A2:Q18"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16:Q18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6301,7 +6301,7 @@
         <v>1661</v>
       </c>
       <c r="C8" s="13">
-        <v>3.0000000000000001E-3</v>
+        <v>0.03</v>
       </c>
       <c r="D8" t="s">
         <v>6</v>
@@ -6313,7 +6313,7 @@
       </c>
       <c r="C9" s="13">
         <f>C7+C8</f>
-        <v>8.6924011044683697E-2</v>
+        <v>0.11392401104468369</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.35">
@@ -6330,7 +6330,7 @@
       </c>
       <c r="C11" s="13">
         <f>C9-C10</f>
-        <v>4.6924011044683696E-2</v>
+        <v>7.3924011044683685E-2</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.35">
@@ -6348,7 +6348,7 @@
       </c>
       <c r="C13" s="46">
         <f>C11+C12</f>
-        <v>6.9763011044683701E-2</v>
+        <v>9.6763011044683683E-2</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -6459,12 +6459,12 @@
         <v>8.3924011044683694E-2</v>
       </c>
       <c r="L18" s="39">
-        <f t="shared" si="0"/>
-        <v>3.0000000000000001E-3</v>
+        <f>VLOOKUP(L17,$B$2:$C$13,2,0)</f>
+        <v>0.03</v>
       </c>
       <c r="M18" s="39">
         <f t="shared" si="0"/>
-        <v>8.6924011044683697E-2</v>
+        <v>0.11392401104468369</v>
       </c>
       <c r="N18" s="39">
         <f t="shared" si="0"/>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="O18" s="39">
         <f t="shared" si="0"/>
-        <v>4.6924011044683696E-2</v>
+        <v>7.3924011044683685E-2</v>
       </c>
       <c r="P18" s="39">
         <f t="shared" si="0"/>
@@ -6480,7 +6480,7 @@
       </c>
       <c r="Q18" s="44">
         <f t="shared" si="0"/>
-        <v>6.9763011044683701E-2</v>
+        <v>9.6763011044683683E-2</v>
       </c>
     </row>
   </sheetData>
@@ -39071,8 +39071,8 @@
   </sheetPr>
   <dimension ref="B2:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13:J14"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>